<commit_message>
agregue 811 epic original
</commit_message>
<xml_diff>
--- a/Competencia DAI/Registro de experimentos.xlsx
+++ b/Competencia DAI/Registro de experimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Desktop\MCD - Laboratorio\7.Labo_1\labo2021DAI\Competencia DAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37740BB-A0B2-4D6E-9C30-843C4774FC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25897056-6324-47B4-B335-FABCC0CC379A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,6 +49,7 @@
     <author>tc={1D7AFF3A-17BA-4E00-B823-8A4202F29845}</author>
     <author>tc={8DEF77AC-D4B1-4465-831F-72EF1E6C0103}</author>
     <author>tc={3D2DA060-6A90-43AE-8406-DC0182BEEB38}</author>
+    <author>tc={138F94E3-E8AF-4A2B-ADC7-B6BDC3FD29BA}</author>
   </authors>
   <commentList>
     <comment ref="O33" authorId="0" shapeId="0" xr:uid="{6F308F7E-C2D1-4436-ADA8-DD7A4F287148}">
@@ -179,12 +180,20 @@
     enviando 11000 registros y no con prob de corte</t>
       </text>
     </comment>
+    <comment ref="AM52" authorId="16" shapeId="0" xr:uid="{138F94E3-E8AF-4A2B-ADC7-B6BDC3FD29BA}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    enviando 11000 registros y no con prob de corte</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="112">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -608,7 +617,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1311,11 +1320,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1690,6 +1699,9 @@
   <threadedComment ref="AM51" dT="2021-10-15T13:30:56.60" personId="{F9B2D9AF-929F-4914-8BC8-9B169E9798E7}" id="{3D2DA060-6A90-43AE-8406-DC0182BEEB38}">
     <text>enviando 11000 registros y no con prob de corte</text>
   </threadedComment>
+  <threadedComment ref="AM52" dT="2021-10-15T13:30:56.60" personId="{F9B2D9AF-929F-4914-8BC8-9B169E9798E7}" id="{138F94E3-E8AF-4A2B-ADC7-B6BDC3FD29BA}">
+    <text>enviando 11000 registros y no con prob de corte</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1698,10 +1710,10 @@
   <dimension ref="A1:AU57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="T33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="AM52" sqref="AM52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6020,194 +6032,216 @@
       <c r="AN50" s="39"/>
     </row>
     <row r="51" spans="1:40" s="107" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" s="82" t="s">
+      <c r="B51" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="E51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="22">
+      <c r="E51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="116">
         <v>4.4537110766522801E-2</v>
       </c>
-      <c r="G51" s="23" t="s">
+      <c r="G51" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H51" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="I51" s="82" t="s">
+      <c r="I51" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="J51" s="82">
+      <c r="J51" s="115">
         <v>11</v>
       </c>
-      <c r="K51" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="L51" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="M51" s="21">
+      <c r="K51" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="M51" s="115">
         <v>202011</v>
       </c>
-      <c r="N51" s="108"/>
-      <c r="O51" s="108"/>
-      <c r="P51" s="108"/>
-      <c r="Q51" s="25"/>
-      <c r="R51" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="S51" s="82" t="s">
+      <c r="N51" s="118"/>
+      <c r="O51" s="118"/>
+      <c r="P51" s="118"/>
+      <c r="Q51" s="120"/>
+      <c r="R51" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="S51" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="T51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="U51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="V51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="W51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="X51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA51" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB51" s="22"/>
-      <c r="AC51" s="20">
+      <c r="T51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="U51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="V51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="W51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="X51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA51" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB51" s="116"/>
+      <c r="AC51" s="113">
         <v>4</v>
       </c>
-      <c r="AD51" s="22">
+      <c r="AD51" s="116">
         <v>150</v>
       </c>
-      <c r="AE51" s="20">
+      <c r="AE51" s="113">
         <v>256</v>
       </c>
-      <c r="AF51" s="21">
+      <c r="AF51" s="115">
         <v>8</v>
       </c>
-      <c r="AG51" s="22">
+      <c r="AG51" s="116">
         <v>300</v>
       </c>
-      <c r="AI51" s="26"/>
-      <c r="AJ51" s="132">
+      <c r="AH51" s="121"/>
+      <c r="AI51" s="122"/>
+      <c r="AJ51" s="123">
         <v>0</v>
       </c>
-      <c r="AK51" s="132">
+      <c r="AK51" s="123">
         <v>57</v>
       </c>
-      <c r="AL51" s="133">
+      <c r="AL51" s="125">
         <v>7.3087499999999999</v>
       </c>
-      <c r="AM51" s="133">
+      <c r="AM51" s="125">
         <v>25.246459999999999</v>
       </c>
-      <c r="AN51" s="39"/>
+      <c r="AN51" s="126"/>
     </row>
     <row r="52" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="112" t="s">
         <v>111</v>
       </c>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
-      <c r="H52" s="20" t="s">
+      <c r="B52" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="E52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="F52" s="115">
+        <v>4.9532710280373801E-2</v>
+      </c>
+      <c r="G52" s="132" t="s">
+        <v>65</v>
+      </c>
+      <c r="H52" s="113" t="s">
         <v>107</v>
       </c>
-      <c r="I52" s="82" t="s">
+      <c r="I52" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="J52" s="82">
+      <c r="J52" s="115">
         <v>32</v>
       </c>
-      <c r="K52" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="L52" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="M52" s="21">
+      <c r="K52" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="L52" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="M52" s="115">
         <v>202011</v>
       </c>
-      <c r="N52" s="108"/>
-      <c r="O52" s="108"/>
-      <c r="P52" s="108"/>
-      <c r="Q52" s="109"/>
-      <c r="R52" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="S52" s="82" t="s">
+      <c r="N52" s="118"/>
+      <c r="O52" s="118"/>
+      <c r="P52" s="118"/>
+      <c r="Q52" s="133"/>
+      <c r="R52" s="113" t="s">
+        <v>41</v>
+      </c>
+      <c r="S52" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="T52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="U52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="V52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="W52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="X52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA52" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB52" s="22"/>
-      <c r="AC52" s="20">
+      <c r="T52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="U52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="V52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="W52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="X52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA52" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB52" s="116"/>
+      <c r="AC52" s="113">
         <v>4</v>
       </c>
-      <c r="AD52" s="22">
+      <c r="AD52" s="116">
         <v>150</v>
       </c>
-      <c r="AE52" s="20">
+      <c r="AE52" s="113">
         <v>256</v>
       </c>
-      <c r="AF52" s="21">
+      <c r="AF52" s="115">
         <v>8</v>
       </c>
-      <c r="AG52" s="22">
+      <c r="AG52" s="116">
         <v>300</v>
       </c>
-      <c r="AI52" s="26"/>
-      <c r="AJ52" s="132"/>
-      <c r="AK52" s="132"/>
-      <c r="AL52" s="133"/>
-      <c r="AM52" s="133"/>
-      <c r="AN52" s="39"/>
+      <c r="AH52" s="121"/>
+      <c r="AI52" s="122"/>
+      <c r="AJ52" s="123">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="123">
+        <v>25</v>
+      </c>
+      <c r="AL52" s="125">
+        <v>7.4637500000000001</v>
+      </c>
+      <c r="AM52" s="125">
+        <v>25.371459999999999</v>
+      </c>
+      <c r="AN52" s="126"/>
     </row>
     <row r="53" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="107"/>

</xml_diff>